<commit_message>
BB0108 EmailSendingBatch - A new batch.
</commit_message>
<xml_diff>
--- a/skrum_docs/02_SpecificationDocs/BATCHList.xlsx
+++ b/skrum_docs/02_SpecificationDocs/BATCHList.xlsx
@@ -316,35 +316,35 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>AchievementRateNoticeMailCommand</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>PostNoticeMailCommand</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>AchievementRegisterReminderMailCommand</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>MemberReportMailCommand</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>GroupReportMailCommand</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>FeedbackTargetReportMailCommand</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ServiceNotificationMailCommand</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>SendMailCommand</t>
+    <t>EmailSendingCommand</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AchievementRateNoticeEmailCommand</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PostNoticeEmailCommand</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AchievementRegisterReminderEmailCommand</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MemberReportEmailCommand</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GroupReportEmailCommand</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FeedbackTargetReportEmailCommand</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ServiceNotificationEmailCommand</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1746,7 +1746,7 @@
         <v>44</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J6" s="16"/>
       <c r="K6" s="18"/>
@@ -1777,7 +1777,7 @@
         <v>44</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J7" s="16"/>
       <c r="K7" s="18"/>
@@ -1810,7 +1810,7 @@
         <v>44</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J8" s="16"/>
       <c r="K8" s="18"/>
@@ -1843,7 +1843,7 @@
         <v>44</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J9" s="16"/>
       <c r="K9" s="18"/>
@@ -1876,7 +1876,7 @@
         <v>44</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J10" s="16"/>
       <c r="K10" s="20"/>
@@ -1909,7 +1909,7 @@
         <v>44</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J11" s="16"/>
       <c r="K11" s="18"/>
@@ -1940,7 +1940,7 @@
         <v>44</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J12" s="16"/>
       <c r="K12" s="18"/>
@@ -1973,7 +1973,7 @@
         <v>44</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J13" s="16"/>
       <c r="K13" s="18"/>

</xml_diff>

<commit_message>
BB0104 MemberAchievementRateReport - A new batch.
</commit_message>
<xml_diff>
--- a/skrum_docs/02_SpecificationDocs/BATCHList.xlsx
+++ b/skrum_docs/02_SpecificationDocs/BATCHList.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
   <si>
     <t>#</t>
     <phoneticPr fontId="1"/>
@@ -332,19 +332,23 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>GroupReportEmailCommand</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FeedbackTargetReportEmailCommand</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ServiceNotificationEmailCommand</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>MemberReportEmailCommand</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>GroupReportEmailCommand</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>FeedbackTargetReportEmailCommand</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ServiceNotificationEmailCommand</t>
+    <t>0, 3, 9</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1843,9 +1847,11 @@
         <v>44</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="J9" s="16"/>
+        <v>54</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>8</v>
+      </c>
       <c r="K9" s="18"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -1876,7 +1882,7 @@
         <v>44</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J10" s="16"/>
       <c r="K10" s="20"/>
@@ -1909,7 +1915,7 @@
         <v>44</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J11" s="16"/>
       <c r="K11" s="18"/>
@@ -1940,7 +1946,7 @@
         <v>44</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J12" s="16"/>
       <c r="K12" s="18"/>
@@ -1970,12 +1976,14 @@
         <v>42</v>
       </c>
       <c r="H13" s="21" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="I13" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="J13" s="16"/>
+      <c r="J13" s="16" t="s">
+        <v>8</v>
+      </c>
       <c r="K13" s="18"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
BB0106 FeedbackTargetReportEmail - A new batch.
</commit_message>
<xml_diff>
--- a/skrum_docs/02_SpecificationDocs/BATCHList.xlsx
+++ b/skrum_docs/02_SpecificationDocs/BATCHList.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
   <si>
     <t>#</t>
     <phoneticPr fontId="1"/>
@@ -1917,7 +1917,9 @@
       <c r="I11" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="J11" s="16"/>
+      <c r="J11" s="16" t="s">
+        <v>8</v>
+      </c>
       <c r="K11" s="18"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
GroupReportEmailBatch - A new batch.
</commit_message>
<xml_diff>
--- a/skrum_docs/02_SpecificationDocs/BATCHList.xlsx
+++ b/skrum_docs/02_SpecificationDocs/BATCHList.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="56">
   <si>
     <t>#</t>
     <phoneticPr fontId="1"/>
@@ -1886,7 +1886,9 @@
       <c r="I10" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="J10" s="16"/>
+      <c r="J10" s="16" t="s">
+        <v>8</v>
+      </c>
       <c r="K10" s="20"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ChangeRole - Changed response interface and revised other bugs.
</commit_message>
<xml_diff>
--- a/skrum_docs/02_SpecificationDocs/BATCHList.xlsx
+++ b/skrum_docs/02_SpecificationDocs/BATCHList.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="62">
   <si>
     <t>#</t>
     <phoneticPr fontId="1"/>
@@ -379,6 +379,10 @@
   </si>
   <si>
     <t>0, 3, 9</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mail_sending</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2055,7 +2059,7 @@
         <v>35</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="H14" s="21" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
Added a new EmailBatch which is DeadlineReminderEmail.
</commit_message>
<xml_diff>
--- a/skrum_docs/02_SpecificationDocs/BATCHList.xlsx
+++ b/skrum_docs/02_SpecificationDocs/BATCHList.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="62">
   <si>
     <t>#</t>
     <phoneticPr fontId="1"/>
@@ -365,27 +365,27 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>進捗登録リマインドメール</t>
+    <t>OkrDeadlineReminderEmailCommand</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>目標期限日リマインダーメール</t>
+    <rPh sb="0" eb="2">
+      <t>モクヒョ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>キゲn</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ビ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>進捗登録リマインダーメール</t>
     <rPh sb="0" eb="4">
       <t>シンチョk</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>目標期限日リマインドメール</t>
-    <rPh sb="0" eb="2">
-      <t>モクヒョ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>キゲn</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>ビ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>DeadlineReminderEmailCommand</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -600,7 +600,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -665,6 +665,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
@@ -1004,12 +1007,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="1" max="1" width="5.5" customWidth="1"/>
     <col min="2" max="2" width="13" style="12" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
-    <col min="5" max="5" width="48.42578125" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="5" max="5" width="48.5" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -1671,15 +1674,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="4.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="4.1640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="18" style="3" customWidth="1"/>
-    <col min="4" max="4" width="41.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="3" customWidth="1"/>
-    <col min="7" max="8" width="18.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="42.28515625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="17"/>
+    <col min="4" max="4" width="41.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="3" customWidth="1"/>
+    <col min="7" max="8" width="18.83203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="42.33203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="38" x14ac:dyDescent="0.55000000000000004">
@@ -1814,11 +1817,14 @@
       <c r="H6" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="I6" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="J6" s="27"/>
-      <c r="K6" s="16"/>
+      <c r="I6" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="28"/>
+      <c r="L6" s="19"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="23">
@@ -1850,8 +1856,9 @@
       </c>
       <c r="J7" s="26"/>
       <c r="K7" s="18"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L7" s="19"/>
+    </row>
+    <row r="8" spans="1:12" ht="40" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1864,7 +1871,7 @@
         <v>19</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>28</v>
@@ -1956,7 +1963,7 @@
       </c>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="40" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <f t="shared" si="0"/>
         <v>7</v>

</xml_diff>